<commit_message>
Tabelas Fato e Dimensao
</commit_message>
<xml_diff>
--- a/Dados/CadastroLojas.xlsx
+++ b/Dados/CadastroLojas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hashtagtreinamentos-my.sharepoint.com/personal/diego_hashtagtreinamentos_com/Documents/Hashtag/Cursos/Aulas Power BI/Power BI Impressionador 2.0/Bases de Dados/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coelh\Pessoal\TI\CURSOS\Hashtag\PowerBICompleto\Aulas\Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="98" documentId="11_AD4D361C20488DEA4E38A031A49E73DA5ADEDD8F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2C6EB87-1AA8-4BC1-835C-240147070621}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0FA8CE-2461-4BB4-AB72-9FE3FF6803C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -2215,20 +2215,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G307"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A295" workbookViewId="0">
-      <selection activeCell="C305" sqref="C305"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2251,7 +2249,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2274,7 +2272,7 @@
         <v>666418406</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2297,7 +2295,7 @@
         <v>782269727</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2320,7 +2318,7 @@
         <v>566476645</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2343,7 +2341,7 @@
         <v>598832615</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2366,7 +2364,7 @@
         <v>200191505</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2389,7 +2387,7 @@
         <v>258070696</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2412,7 +2410,7 @@
         <v>137257008</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2435,7 +2433,7 @@
         <v>148283535</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2458,7 +2456,7 @@
         <v>757556625</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2481,7 +2479,7 @@
         <v>772151648</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2504,7 +2502,7 @@
         <v>438015135</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>13</v>
       </c>
@@ -2527,7 +2525,7 @@
         <v>458643508</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>14</v>
       </c>
@@ -2550,7 +2548,7 @@
         <v>293551216</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>15</v>
       </c>
@@ -2573,7 +2571,7 @@
         <v>150585293</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>16</v>
       </c>
@@ -2596,7 +2594,7 @@
         <v>682882258</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>17</v>
       </c>
@@ -2619,7 +2617,7 @@
         <v>216921175</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>18</v>
       </c>
@@ -2642,7 +2640,7 @@
         <v>550162476</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>20</v>
       </c>
@@ -2665,7 +2663,7 @@
         <v>622602258</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>21</v>
       </c>
@@ -2688,7 +2686,7 @@
         <v>658086597</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>22</v>
       </c>
@@ -2711,7 +2709,7 @@
         <v>398404937</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>23</v>
       </c>
@@ -2734,7 +2732,7 @@
         <v>283231970</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>24</v>
       </c>
@@ -2757,7 +2755,7 @@
         <v>496323922</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>25</v>
       </c>
@@ -2780,7 +2778,7 @@
         <v>391200910</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>26</v>
       </c>
@@ -2803,7 +2801,7 @@
         <v>517979422</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>27</v>
       </c>
@@ -2826,7 +2824,7 @@
         <v>958599604</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>28</v>
       </c>
@@ -2849,7 +2847,7 @@
         <v>383187294</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>30</v>
       </c>
@@ -2872,7 +2870,7 @@
         <v>710773314</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>31</v>
       </c>
@@ -2895,7 +2893,7 @@
         <v>703600407</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>32</v>
       </c>
@@ -2918,7 +2916,7 @@
         <v>656196435</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>33</v>
       </c>
@@ -2941,7 +2939,7 @@
         <v>725440447</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>34</v>
       </c>
@@ -2964,7 +2962,7 @@
         <v>192837467</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>35</v>
       </c>
@@ -2987,7 +2985,7 @@
         <v>126592536</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>36</v>
       </c>
@@ -3010,7 +3008,7 @@
         <v>137497733</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>37</v>
       </c>
@@ -3033,7 +3031,7 @@
         <v>637536440</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>38</v>
       </c>
@@ -3056,7 +3054,7 @@
         <v>459664769</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>39</v>
       </c>
@@ -3079,7 +3077,7 @@
         <v>820819434</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>40</v>
       </c>
@@ -3102,7 +3100,7 @@
         <v>535707685</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>41</v>
       </c>
@@ -3125,7 +3123,7 @@
         <v>233971955</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>42</v>
       </c>
@@ -3148,7 +3146,7 @@
         <v>784596643</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>43</v>
       </c>
@@ -3171,7 +3169,7 @@
         <v>148808289</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>44</v>
       </c>
@@ -3194,7 +3192,7 @@
         <v>350727716</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>45</v>
       </c>
@@ -3217,7 +3215,7 @@
         <v>472025954</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>46</v>
       </c>
@@ -3240,7 +3238,7 @@
         <v>431015240</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>47</v>
       </c>
@@ -3263,7 +3261,7 @@
         <v>632618369</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>49</v>
       </c>
@@ -3286,7 +3284,7 @@
         <v>648342376</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>50</v>
       </c>
@@ -3309,7 +3307,7 @@
         <v>749372644</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>51</v>
       </c>
@@ -3332,7 +3330,7 @@
         <v>441540643</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>52</v>
       </c>
@@ -3355,7 +3353,7 @@
         <v>442085397</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>53</v>
       </c>
@@ -3378,7 +3376,7 @@
         <v>248831332</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>54</v>
       </c>
@@ -3401,7 +3399,7 @@
         <v>996214585</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>55</v>
       </c>
@@ -3424,7 +3422,7 @@
         <v>676041953</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>57</v>
       </c>
@@ -3447,7 +3445,7 @@
         <v>213808369</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>58</v>
       </c>
@@ -3470,7 +3468,7 @@
         <v>457065191</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>59</v>
       </c>
@@ -3493,7 +3491,7 @@
         <v>443194701</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>60</v>
       </c>
@@ -3516,7 +3514,7 @@
         <v>699395364</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>61</v>
       </c>
@@ -3539,7 +3537,7 @@
         <v>274064609</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>63</v>
       </c>
@@ -3562,7 +3560,7 @@
         <v>395943763</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>64</v>
       </c>
@@ -3585,7 +3583,7 @@
         <v>533133364</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>65</v>
       </c>
@@ -3608,7 +3606,7 @@
         <v>922690535</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>66</v>
       </c>
@@ -3631,7 +3629,7 @@
         <v>650601944</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>67</v>
       </c>
@@ -3654,7 +3652,7 @@
         <v>580812912</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>68</v>
       </c>
@@ -3677,7 +3675,7 @@
         <v>334539089</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>69</v>
       </c>
@@ -3700,7 +3698,7 @@
         <v>291633377</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>70</v>
       </c>
@@ -3723,7 +3721,7 @@
         <v>815484901</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>71</v>
       </c>
@@ -3746,7 +3744,7 @@
         <v>113671049</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>72</v>
       </c>
@@ -3769,7 +3767,7 @@
         <v>724498251</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>73</v>
       </c>
@@ -3792,7 +3790,7 @@
         <v>674519288</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>74</v>
       </c>
@@ -3815,7 +3813,7 @@
         <v>279794445</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>75</v>
       </c>
@@ -3838,7 +3836,7 @@
         <v>472995633</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>76</v>
       </c>
@@ -3861,7 +3859,7 @@
         <v>776364792</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>77</v>
       </c>
@@ -3884,7 +3882,7 @@
         <v>397915178</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>78</v>
       </c>
@@ -3907,7 +3905,7 @@
         <v>495088235</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>79</v>
       </c>
@@ -3930,7 +3928,7 @@
         <v>772206299</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>80</v>
       </c>
@@ -3953,7 +3951,7 @@
         <v>576077763</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>81</v>
       </c>
@@ -3976,7 +3974,7 @@
         <v>686988860</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>82</v>
       </c>
@@ -3999,7 +3997,7 @@
         <v>532507973</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>83</v>
       </c>
@@ -4022,7 +4020,7 @@
         <v>867570901</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>85</v>
       </c>
@@ -4045,7 +4043,7 @@
         <v>610684796</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>86</v>
       </c>
@@ -4068,7 +4066,7 @@
         <v>285197952</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>87</v>
       </c>
@@ -4091,7 +4089,7 @@
         <v>195827168</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>88</v>
       </c>
@@ -4114,7 +4112,7 @@
         <v>809496425</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>89</v>
       </c>
@@ -4137,7 +4135,7 @@
         <v>514178779</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>90</v>
       </c>
@@ -4160,7 +4158,7 @@
         <v>461667762</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>91</v>
       </c>
@@ -4183,7 +4181,7 @@
         <v>774637903</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>92</v>
       </c>
@@ -4206,7 +4204,7 @@
         <v>481194799</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>93</v>
       </c>
@@ -4229,7 +4227,7 @@
         <v>339644249</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>94</v>
       </c>
@@ -4252,7 +4250,7 @@
         <v>210018045</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>95</v>
       </c>
@@ -4275,7 +4273,7 @@
         <v>642112421</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>96</v>
       </c>
@@ -4298,7 +4296,7 @@
         <v>483669359</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>97</v>
       </c>
@@ -4321,7 +4319,7 @@
         <v>809793860</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>98</v>
       </c>
@@ -4344,7 +4342,7 @@
         <v>633400076</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>99</v>
       </c>
@@ -4367,7 +4365,7 @@
         <v>341549666</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>100</v>
       </c>
@@ -4390,7 +4388,7 @@
         <v>129109320</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>101</v>
       </c>
@@ -4413,7 +4411,7 @@
         <v>665062470</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>102</v>
       </c>
@@ -4436,7 +4434,7 @@
         <v>123278813</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>103</v>
       </c>
@@ -4459,7 +4457,7 @@
         <v>689760739</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>104</v>
       </c>
@@ -4482,7 +4480,7 @@
         <v>616610071</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>105</v>
       </c>
@@ -4505,7 +4503,7 @@
         <v>610522609</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>107</v>
       </c>
@@ -4528,7 +4526,7 @@
         <v>173308423</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>108</v>
       </c>
@@ -4551,7 +4549,7 @@
         <v>420751339</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>109</v>
       </c>
@@ -4574,7 +4572,7 @@
         <v>906150265</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>110</v>
       </c>
@@ -4597,7 +4595,7 @@
         <v>765360121</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>111</v>
       </c>
@@ -4620,7 +4618,7 @@
         <v>247711041</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>113</v>
       </c>
@@ -4643,7 +4641,7 @@
         <v>965667424</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>114</v>
       </c>
@@ -4666,7 +4664,7 @@
         <v>869021433</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>115</v>
       </c>
@@ -4689,7 +4687,7 @@
         <v>645880466</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>116</v>
       </c>
@@ -4712,7 +4710,7 @@
         <v>146422074</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>117</v>
       </c>
@@ -4735,7 +4733,7 @@
         <v>561731073</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>118</v>
       </c>
@@ -4758,7 +4756,7 @@
         <v>405403135</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>120</v>
       </c>
@@ -4781,7 +4779,7 @@
         <v>475046314</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>121</v>
       </c>
@@ -4804,7 +4802,7 @@
         <v>297881149</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>122</v>
       </c>
@@ -4827,7 +4825,7 @@
         <v>485593871</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>123</v>
       </c>
@@ -4850,7 +4848,7 @@
         <v>302242532</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>124</v>
       </c>
@@ -4873,7 +4871,7 @@
         <v>522461326</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>125</v>
       </c>
@@ -4896,7 +4894,7 @@
         <v>952026498</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>126</v>
       </c>
@@ -4919,7 +4917,7 @@
         <v>517595382</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>127</v>
       </c>
@@ -4942,7 +4940,7 @@
         <v>980680625</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>128</v>
       </c>
@@ -4965,7 +4963,7 @@
         <v>247362571</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>130</v>
       </c>
@@ -4988,7 +4986,7 @@
         <v>337265534</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>131</v>
       </c>
@@ -5011,7 +5009,7 @@
         <v>680232999</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>132</v>
       </c>
@@ -5034,7 +5032,7 @@
         <v>372466625</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>133</v>
       </c>
@@ -5057,7 +5055,7 @@
         <v>641555206</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>134</v>
       </c>
@@ -5080,7 +5078,7 @@
         <v>786504524</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>135</v>
       </c>
@@ -5103,7 +5101,7 @@
         <v>571114764</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>136</v>
       </c>
@@ -5126,7 +5124,7 @@
         <v>148151205</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>137</v>
       </c>
@@ -5149,7 +5147,7 @@
         <v>574406867</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>138</v>
       </c>
@@ -5172,7 +5170,7 @@
         <v>336784632</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>139</v>
       </c>
@@ -5195,7 +5193,7 @@
         <v>290113089</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>140</v>
       </c>
@@ -5218,7 +5216,7 @@
         <v>353807270</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>141</v>
       </c>
@@ -5241,7 +5239,7 @@
         <v>346798696</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>142</v>
       </c>
@@ -5264,7 +5262,7 @@
         <v>137393586</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>143</v>
       </c>
@@ -5287,7 +5285,7 @@
         <v>961927762</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>144</v>
       </c>
@@ -5310,7 +5308,7 @@
         <v>254510322</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>145</v>
       </c>
@@ -5333,7 +5331,7 @@
         <v>887571364</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>146</v>
       </c>
@@ -5356,7 +5354,7 @@
         <v>932366227</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>147</v>
       </c>
@@ -5379,7 +5377,7 @@
         <v>223486932</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>149</v>
       </c>
@@ -5402,7 +5400,7 @@
         <v>627650321</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>150</v>
       </c>
@@ -5425,7 +5423,7 @@
         <v>876032050</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>151</v>
       </c>
@@ -5448,7 +5446,7 @@
         <v>937038287</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>152</v>
       </c>
@@ -5471,7 +5469,7 @@
         <v>306037861</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>153</v>
       </c>
@@ -5494,7 +5492,7 @@
         <v>803704632</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>154</v>
       </c>
@@ -5517,7 +5515,7 @@
         <v>379241392</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>155</v>
       </c>
@@ -5540,7 +5538,7 @@
         <v>358847436</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>156</v>
       </c>
@@ -5563,7 +5561,7 @@
         <v>70061570</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>157</v>
       </c>
@@ -5586,7 +5584,7 @@
         <v>630411291</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>158</v>
       </c>
@@ -5609,7 +5607,7 @@
         <v>126341752</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>159</v>
       </c>
@@ -5632,7 +5630,7 @@
         <v>344952472</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>160</v>
       </c>
@@ -5655,7 +5653,7 @@
         <v>945824923</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>161</v>
       </c>
@@ -5678,7 +5676,7 @@
         <v>813900107</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>163</v>
       </c>
@@ -5701,7 +5699,7 @@
         <v>546842302</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>164</v>
       </c>
@@ -5724,7 +5722,7 @@
         <v>376237087</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>165</v>
       </c>
@@ -5747,7 +5745,7 @@
         <v>264003477</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>166</v>
       </c>
@@ -5770,7 +5768,7 @@
         <v>525693146</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>167</v>
       </c>
@@ -5793,7 +5791,7 @@
         <v>720094732</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>168</v>
       </c>
@@ -5816,7 +5814,7 @@
         <v>907267425</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>169</v>
       </c>
@@ -5839,7 +5837,7 @@
         <v>986345837</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>170</v>
       </c>
@@ -5862,7 +5860,7 @@
         <v>467060037</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>171</v>
       </c>
@@ -5885,7 +5883,7 @@
         <v>825644232</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>172</v>
       </c>
@@ -5908,7 +5906,7 @@
         <v>173998548</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>173</v>
       </c>
@@ -5931,7 +5929,7 @@
         <v>196398360</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>174</v>
       </c>
@@ -5954,7 +5952,7 @@
         <v>456413934</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>175</v>
       </c>
@@ -5977,7 +5975,7 @@
         <v>138379506</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>176</v>
       </c>
@@ -6000,7 +5998,7 @@
         <v>395450339</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>177</v>
       </c>
@@ -6023,7 +6021,7 @@
         <v>263712841</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>178</v>
       </c>
@@ -6046,7 +6044,7 @@
         <v>796622820</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>179</v>
       </c>
@@ -6069,7 +6067,7 @@
         <v>589421831</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>180</v>
       </c>
@@ -6092,7 +6090,7 @@
         <v>369380564</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>181</v>
       </c>
@@ -6115,7 +6113,7 @@
         <v>306512818</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>182</v>
       </c>
@@ -6138,7 +6136,7 @@
         <v>457755197</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>183</v>
       </c>
@@ -6161,7 +6159,7 @@
         <v>203408476</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>185</v>
       </c>
@@ -6184,7 +6182,7 @@
         <v>188310691</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>186</v>
       </c>
@@ -6207,7 +6205,7 @@
         <v>601669174</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>187</v>
       </c>
@@ -6230,7 +6228,7 @@
         <v>906706359</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>188</v>
       </c>
@@ -6253,7 +6251,7 @@
         <v>348508241</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>189</v>
       </c>
@@ -6276,7 +6274,7 @@
         <v>783213370</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>190</v>
       </c>
@@ -6299,7 +6297,7 @@
         <v>848395427</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>191</v>
       </c>
@@ -6322,7 +6320,7 @@
         <v>299075214</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>192</v>
       </c>
@@ -6345,7 +6343,7 @@
         <v>985694474</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>193</v>
       </c>
@@ -6368,7 +6366,7 @@
         <v>444098003</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>194</v>
       </c>
@@ -6391,7 +6389,7 @@
         <v>374562531</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>195</v>
       </c>
@@ -6414,7 +6412,7 @@
         <v>894518598</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>196</v>
       </c>
@@ -6437,7 +6435,7 @@
         <v>949277479</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>197</v>
       </c>
@@ -6460,7 +6458,7 @@
         <v>258989109</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>198</v>
       </c>
@@ -6483,7 +6481,7 @@
         <v>125725480</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>201</v>
       </c>
@@ -6506,7 +6504,7 @@
         <v>79894784</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>202</v>
       </c>
@@ -6529,7 +6527,7 @@
         <v>24501346</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>203</v>
       </c>
@@ -6552,7 +6550,7 @@
         <v>60561942</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>204</v>
       </c>
@@ -6575,7 +6573,7 @@
         <v>19022472</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>205</v>
       </c>
@@ -6598,7 +6596,7 @@
         <v>25909892</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>206</v>
       </c>
@@ -6621,7 +6619,7 @@
         <v>20664168</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>207</v>
       </c>
@@ -6644,7 +6642,7 @@
         <v>86141359</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>208</v>
       </c>
@@ -6667,7 +6665,7 @@
         <v>87233411</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>209</v>
       </c>
@@ -6690,7 +6688,7 @@
         <v>59736745</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>210</v>
       </c>
@@ -6713,7 +6711,7 @@
         <v>49013455</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>211</v>
       </c>
@@ -6736,7 +6734,7 @@
         <v>11800128</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>212</v>
       </c>
@@ -6759,7 +6757,7 @@
         <v>55703788</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>213</v>
       </c>
@@ -6782,7 +6780,7 @@
         <v>40187876</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>214</v>
       </c>
@@ -6805,7 +6803,7 @@
         <v>51209286</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>215</v>
       </c>
@@ -6828,7 +6826,7 @@
         <v>83707979</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>216</v>
       </c>
@@ -6851,7 +6849,7 @@
         <v>41958108</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>217</v>
       </c>
@@ -6874,7 +6872,7 @@
         <v>28401446</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>218</v>
       </c>
@@ -6897,7 +6895,7 @@
         <v>79406455</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>219</v>
       </c>
@@ -6920,7 +6918,7 @@
         <v>55804439</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>220</v>
       </c>
@@ -6943,7 +6941,7 @@
         <v>16642888</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>221</v>
       </c>
@@ -6966,7 +6964,7 @@
         <v>76455457</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>222</v>
       </c>
@@ -6989,7 +6987,7 @@
         <v>58821163</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>223</v>
       </c>
@@ -7012,7 +7010,7 @@
         <v>19021172</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>224</v>
       </c>
@@ -7035,7 +7033,7 @@
         <v>13417898</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>225</v>
       </c>
@@ -7058,7 +7056,7 @@
         <v>71821223</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>226</v>
       </c>
@@ -7081,7 +7079,7 @@
         <v>12389226</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>227</v>
       </c>
@@ -7104,7 +7102,7 @@
         <v>248819362</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>228</v>
       </c>
@@ -7127,7 +7125,7 @@
         <v>73120635</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>230</v>
       </c>
@@ -7150,7 +7148,7 @@
         <v>62579514</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>231</v>
       </c>
@@ -7173,7 +7171,7 @@
         <v>18038468</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>232</v>
       </c>
@@ -7196,7 +7194,7 @@
         <v>83696351</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>233</v>
       </c>
@@ -7219,7 +7217,7 @@
         <v>48833603</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>234</v>
       </c>
@@ -7242,7 +7240,7 @@
         <v>26394472</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>235</v>
       </c>
@@ -7265,7 +7263,7 @@
         <v>82817771</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>236</v>
       </c>
@@ -7288,7 +7286,7 @@
         <v>72356048</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>237</v>
       </c>
@@ -7311,7 +7309,7 @@
         <v>16270597</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>238</v>
       </c>
@@ -7334,7 +7332,7 @@
         <v>52637305</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>239</v>
       </c>
@@ -7357,7 +7355,7 @@
         <v>43142456</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>240</v>
       </c>
@@ -7380,7 +7378,7 @@
         <v>56321814</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>241</v>
       </c>
@@ -7403,7 +7401,7 @@
         <v>61982286</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>242</v>
       </c>
@@ -7426,7 +7424,7 @@
         <v>74247008</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>243</v>
       </c>
@@ -7449,7 +7447,7 @@
         <v>39004245</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>244</v>
       </c>
@@ -7472,7 +7470,7 @@
         <v>77433755</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>245</v>
       </c>
@@ -7495,7 +7493,7 @@
         <v>71454845</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>246</v>
       </c>
@@ -7518,7 +7516,7 @@
         <v>32438821</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>247</v>
       </c>
@@ -7541,7 +7539,7 @@
         <v>32274060</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>248</v>
       </c>
@@ -7564,7 +7562,7 @@
         <v>36187290</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>249</v>
       </c>
@@ -7587,7 +7585,7 @@
         <v>76116398</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>250</v>
       </c>
@@ -7610,7 +7608,7 @@
         <v>42233596</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>251</v>
       </c>
@@ -7633,7 +7631,7 @@
         <v>650334478</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>252</v>
       </c>
@@ -7656,7 +7654,7 @@
         <v>43862649</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>253</v>
       </c>
@@ -7679,7 +7677,7 @@
         <v>32797595</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>254</v>
       </c>
@@ -7702,7 +7700,7 @@
         <v>774810078</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>255</v>
       </c>
@@ -7725,7 +7723,7 @@
         <v>183725981</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>256</v>
       </c>
@@ -7748,7 +7746,7 @@
         <v>627846759</v>
       </c>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>257</v>
       </c>
@@ -7771,7 +7769,7 @@
         <v>709193971</v>
       </c>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>258</v>
       </c>
@@ -7794,7 +7792,7 @@
         <v>572355419</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>259</v>
       </c>
@@ -7817,7 +7815,7 @@
         <v>386999248</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>260</v>
       </c>
@@ -7840,7 +7838,7 @@
         <v>593618161</v>
       </c>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>261</v>
       </c>
@@ -7863,7 +7861,7 @@
         <v>416343487</v>
       </c>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>262</v>
       </c>
@@ -7886,7 +7884,7 @@
         <v>142234187</v>
       </c>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>263</v>
       </c>
@@ -7909,7 +7907,7 @@
         <v>88518310</v>
       </c>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>264</v>
       </c>
@@ -7932,7 +7930,7 @@
         <v>565563007</v>
       </c>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>265</v>
       </c>
@@ -7955,7 +7953,7 @@
         <v>433152035</v>
       </c>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>267</v>
       </c>
@@ -7978,7 +7976,7 @@
         <v>130225150</v>
       </c>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>268</v>
       </c>
@@ -8001,7 +7999,7 @@
         <v>232987780</v>
       </c>
     </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>269</v>
       </c>
@@ -8024,7 +8022,7 @@
         <v>365068953</v>
       </c>
     </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>270</v>
       </c>
@@ -8047,7 +8045,7 @@
         <v>988529296</v>
       </c>
     </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>271</v>
       </c>
@@ -8070,7 +8068,7 @@
         <v>764017847</v>
       </c>
     </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>272</v>
       </c>
@@ -8093,7 +8091,7 @@
         <v>708971555</v>
       </c>
     </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>273</v>
       </c>
@@ -8116,7 +8114,7 @@
         <v>586281819</v>
       </c>
     </row>
-    <row r="257" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>274</v>
       </c>
@@ -8139,7 +8137,7 @@
         <v>354370458</v>
       </c>
     </row>
-    <row r="258" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>275</v>
       </c>
@@ -8162,7 +8160,7 @@
         <v>595376649</v>
       </c>
     </row>
-    <row r="259" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>276</v>
       </c>
@@ -8185,7 +8183,7 @@
         <v>386040813</v>
       </c>
     </row>
-    <row r="260" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>277</v>
       </c>
@@ -8208,7 +8206,7 @@
         <v>632396771</v>
       </c>
     </row>
-    <row r="261" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>278</v>
       </c>
@@ -8231,7 +8229,7 @@
         <v>250826665</v>
       </c>
     </row>
-    <row r="262" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>279</v>
       </c>
@@ -8254,7 +8252,7 @@
         <v>433505294</v>
       </c>
     </row>
-    <row r="263" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>280</v>
       </c>
@@ -8277,7 +8275,7 @@
         <v>318254527</v>
       </c>
     </row>
-    <row r="264" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>281</v>
       </c>
@@ -8300,7 +8298,7 @@
         <v>197228998</v>
       </c>
     </row>
-    <row r="265" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <v>282</v>
       </c>
@@ -8323,7 +8321,7 @@
         <v>435474140</v>
       </c>
     </row>
-    <row r="266" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <v>283</v>
       </c>
@@ -8346,7 +8344,7 @@
         <v>931840511</v>
       </c>
     </row>
-    <row r="267" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <v>284</v>
       </c>
@@ -8369,7 +8367,7 @@
         <v>512590978</v>
       </c>
     </row>
-    <row r="268" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
         <v>285</v>
       </c>
@@ -8392,7 +8390,7 @@
         <v>513880284</v>
       </c>
     </row>
-    <row r="269" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
         <v>286</v>
       </c>
@@ -8415,7 +8413,7 @@
         <v>499598996</v>
       </c>
     </row>
-    <row r="270" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
         <v>287</v>
       </c>
@@ -8438,7 +8436,7 @@
         <v>492492830</v>
       </c>
     </row>
-    <row r="271" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <v>288</v>
       </c>
@@ -8461,7 +8459,7 @@
         <v>543574368</v>
       </c>
     </row>
-    <row r="272" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <v>289</v>
       </c>
@@ -8484,7 +8482,7 @@
         <v>375784151</v>
       </c>
     </row>
-    <row r="273" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <v>290</v>
       </c>
@@ -8507,7 +8505,7 @@
         <v>909562107</v>
       </c>
     </row>
-    <row r="274" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
         <v>291</v>
       </c>
@@ -8530,7 +8528,7 @@
         <v>893455088</v>
       </c>
     </row>
-    <row r="275" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <v>292</v>
       </c>
@@ -8553,7 +8551,7 @@
         <v>538294690</v>
       </c>
     </row>
-    <row r="276" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
         <v>293</v>
       </c>
@@ -8576,7 +8574,7 @@
         <v>830822258</v>
       </c>
     </row>
-    <row r="277" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
         <v>294</v>
       </c>
@@ -8599,7 +8597,7 @@
         <v>236629633</v>
       </c>
     </row>
-    <row r="278" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
         <v>295</v>
       </c>
@@ -8622,7 +8620,7 @@
         <v>143109286</v>
       </c>
     </row>
-    <row r="279" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
         <v>296</v>
       </c>
@@ -8645,7 +8643,7 @@
         <v>790452312</v>
       </c>
     </row>
-    <row r="280" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
         <v>297</v>
       </c>
@@ -8668,7 +8666,7 @@
         <v>75204155</v>
       </c>
     </row>
-    <row r="281" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
         <v>298</v>
       </c>
@@ -8691,7 +8689,7 @@
         <v>252028569</v>
       </c>
     </row>
-    <row r="282" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A282" s="1">
         <v>299</v>
       </c>
@@ -8714,7 +8712,7 @@
         <v>204116236</v>
       </c>
     </row>
-    <row r="283" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
         <v>300</v>
       </c>
@@ -8737,7 +8735,7 @@
         <v>72489301</v>
       </c>
     </row>
-    <row r="284" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
         <v>301</v>
       </c>
@@ -8760,7 +8758,7 @@
         <v>434515094</v>
       </c>
     </row>
-    <row r="285" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
         <v>302</v>
       </c>
@@ -8783,7 +8781,7 @@
         <v>701312058</v>
       </c>
     </row>
-    <row r="286" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
         <v>303</v>
       </c>
@@ -8806,7 +8804,7 @@
         <v>34233439</v>
       </c>
     </row>
-    <row r="287" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
         <v>304</v>
       </c>
@@ -8829,7 +8827,7 @@
         <v>48204922</v>
       </c>
     </row>
-    <row r="288" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
         <v>305</v>
       </c>
@@ -8852,7 +8850,7 @@
         <v>50980888</v>
       </c>
     </row>
-    <row r="289" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
         <v>12</v>
       </c>
@@ -8875,7 +8873,7 @@
         <v>259222640</v>
       </c>
     </row>
-    <row r="290" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
         <v>19</v>
       </c>
@@ -8898,7 +8896,7 @@
         <v>487302296</v>
       </c>
     </row>
-    <row r="291" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A291" s="1">
         <v>29</v>
       </c>
@@ -8921,7 +8919,7 @@
         <v>820669403</v>
       </c>
     </row>
-    <row r="292" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A292" s="1">
         <v>48</v>
       </c>
@@ -8944,7 +8942,7 @@
         <v>547836166</v>
       </c>
     </row>
-    <row r="293" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A293" s="1">
         <v>62</v>
       </c>
@@ -8967,7 +8965,7 @@
         <v>846721619</v>
       </c>
     </row>
-    <row r="294" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A294" s="1">
         <v>84</v>
       </c>
@@ -8990,7 +8988,7 @@
         <v>852707750</v>
       </c>
     </row>
-    <row r="295" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A295" s="1">
         <v>112</v>
       </c>
@@ -9013,7 +9011,7 @@
         <v>742881528</v>
       </c>
     </row>
-    <row r="296" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A296" s="1">
         <v>119</v>
       </c>
@@ -9036,7 +9034,7 @@
         <v>604090222</v>
       </c>
     </row>
-    <row r="297" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A297" s="1">
         <v>129</v>
       </c>
@@ -9059,7 +9057,7 @@
         <v>989752967</v>
       </c>
     </row>
-    <row r="298" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A298" s="1">
         <v>148</v>
       </c>
@@ -9082,7 +9080,7 @@
         <v>893759247</v>
       </c>
     </row>
-    <row r="299" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A299" s="1">
         <v>162</v>
       </c>
@@ -9105,7 +9103,7 @@
         <v>571434549</v>
       </c>
     </row>
-    <row r="300" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A300" s="1">
         <v>184</v>
       </c>
@@ -9128,7 +9126,7 @@
         <v>778863176</v>
       </c>
     </row>
-    <row r="301" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A301" s="1">
         <v>199</v>
       </c>
@@ -9151,7 +9149,7 @@
         <v>777271114</v>
       </c>
     </row>
-    <row r="302" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A302" s="1">
         <v>200</v>
       </c>
@@ -9174,7 +9172,7 @@
         <v>797635524</v>
       </c>
     </row>
-    <row r="303" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A303" s="1">
         <v>306</v>
       </c>
@@ -9197,7 +9195,7 @@
         <v>18399404</v>
       </c>
     </row>
-    <row r="304" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A304" s="1">
         <v>307</v>
       </c>
@@ -9220,7 +9218,7 @@
         <v>941810292</v>
       </c>
     </row>
-    <row r="305" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A305" s="1">
         <v>308</v>
       </c>
@@ -9243,7 +9241,7 @@
         <v>626023320</v>
       </c>
     </row>
-    <row r="306" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A306" s="1">
         <v>309</v>
       </c>
@@ -9266,7 +9264,7 @@
         <v>58240939</v>
       </c>
     </row>
-    <row r="307" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:7" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A307" s="1">
         <v>310</v>
       </c>

</xml_diff>